<commit_message>
update project 1 grade
</commit_message>
<xml_diff>
--- a/testJS/data/P1_comment.xlsx
+++ b/testJS/data/P1_comment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TTU-CS\Github\CS5331_Spring2019\testJS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5DCAFF-8BB2-4CD5-BBF5-CCF28069F79E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFF2E18-C5EB-402C-AC6B-C9F2BEA97CE3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{D723DA88-2802-4F03-A580-A328A75F80DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{D723DA88-2802-4F03-A580-A328A75F80DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Fullname</t>
   </si>
@@ -196,9 +196,6 @@
     <t>No secondary selection no data finding(-1%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> no data process discussion (-1%)</t>
-  </si>
-  <si>
     <t>P1_code</t>
   </si>
   <si>
@@ -249,6 +246,21 @@
     <t>Found the data online (github)
 No axis labels
 Selection on the text legends, No date filtering. No image description in readme (-0.5)</t>
+  </si>
+  <si>
+    <t>No video (-3), No findings (-1)</t>
+  </si>
+  <si>
+    <t>Late video (-1),late update readme(-1), No Finding (-1)</t>
+  </si>
+  <si>
+    <t>Late image (-0.5), not telling data process (-1), late video (-1), late readme update(-1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no data process discussion (-1%), late video (-1)</t>
+  </si>
+  <si>
+    <t>No data description (-1), failed to show image in readme (-0.5)</t>
   </si>
 </sst>
 </file>
@@ -605,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208C5A55-07FC-406A-B2A4-16AD07183CFF}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,13 +635,13 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -641,6 +653,9 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -681,7 +696,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6">
         <v>11</v>
@@ -703,7 +718,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8">
         <v>9</v>
@@ -766,7 +781,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -790,11 +805,17 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -826,7 +847,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -848,7 +869,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -873,7 +894,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -886,7 +907,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -894,7 +915,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30">
         <v>12</v>
@@ -948,7 +969,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -973,7 +994,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38">
         <v>10</v>
@@ -990,7 +1011,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39">
         <v>12</v>
@@ -1006,6 +1027,9 @@
       <c r="A40" t="s">
         <v>39</v>
       </c>
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1017,7 +1041,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C42">
         <v>9</v>
@@ -1034,7 +1058,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>